<commit_message>
deploy Mysql - Railway
</commit_message>
<xml_diff>
--- a/data/dataset.xlsx
+++ b/data/dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\APP-RF\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Angel\OneDrive\Desktop\Percepcion\APP-RF\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAEF7144-7397-4C1E-B328-034A69B37A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49846DC-C862-413B-BADE-88C353445D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5625" yWindow="2295" windowWidth="14625" windowHeight="13470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="176">
   <si>
     <t>ID</t>
   </si>
@@ -500,6 +500,54 @@
   </si>
   <si>
     <t>jchavezd9@upao.edu.pe</t>
+  </si>
+  <si>
+    <t>Melissa</t>
+  </si>
+  <si>
+    <t>Yengle</t>
+  </si>
+  <si>
+    <t>ayenglem1@upao.edu.pe</t>
+  </si>
+  <si>
+    <t>ISIA/ANDREA_MELISSA/Melissa.jpg</t>
+  </si>
+  <si>
+    <t>Jeisson</t>
+  </si>
+  <si>
+    <t>Espinoza</t>
+  </si>
+  <si>
+    <t>jespinozae2@upao.edu.pe</t>
+  </si>
+  <si>
+    <t>ISIA/JEISSON_AARON/Jeisson.jpg</t>
+  </si>
+  <si>
+    <t>Jonatan</t>
+  </si>
+  <si>
+    <t>Mendoza</t>
+  </si>
+  <si>
+    <t>jmendozaz2@upao.edu.pe</t>
+  </si>
+  <si>
+    <t>ISIA/JONATAN_DEL_PIERO/jonatan.jpeg</t>
+  </si>
+  <si>
+    <t>Joseph</t>
+  </si>
+  <si>
+    <t>Salinas</t>
+  </si>
+  <si>
+    <t>jsalinasr3@upao.edu.pe</t>
+  </si>
+  <si>
+    <t>ISIA/JOSEPH_KEVIN/kev.jpeg</t>
   </si>
 </sst>
 </file>
@@ -578,12 +626,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -889,15 +936,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P32"/>
+  <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -917,8 +964,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>246403</v>
       </c>
       <c r="B2" t="s">
@@ -937,7 +984,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>243425</v>
       </c>
@@ -957,7 +1004,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>259687</v>
       </c>
@@ -977,572 +1024,640 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>253703</v>
+      </c>
+      <c r="B5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>200549</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>21</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>156</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>22</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E6" t="s">
         <v>23</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>1</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>26</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>27</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>28</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>247603</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>30</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>31</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>32</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>33</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>260815</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>35</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>36</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>37</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>38</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>245499</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>40</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>41</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>42</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E10" t="s">
         <v>43</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F10" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>217654</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>45</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>46</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>47</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>48</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>256897</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>50</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>51</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>52</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" t="s">
         <v>53</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F12" t="s">
         <v>54</v>
       </c>
-      <c r="P11" s="4"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="P12" s="3"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>205878</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>55</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>154</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>56</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
         <v>57</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F13" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>237448</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>59</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>60</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>61</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>62</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F14" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>252811</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>64</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>65</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>66</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E15" t="s">
         <v>67</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F15" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>258740</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>69</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>155</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>70</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E16" t="s">
         <v>71</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F16" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>260175</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>73</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>74</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>75</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" t="s">
         <v>76</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F17" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>258658</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>78</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>79</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" t="s">
         <v>80</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F18" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>241130</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>82</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>83</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>84</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E19" t="s">
         <v>85</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F19" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>261349</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>87</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>157</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E20" t="s">
         <v>88</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F20" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>268437</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>90</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>91</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>92</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E21" t="s">
         <v>93</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F21" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>261701</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>95</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>96</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D22" t="s">
         <v>97</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E22" t="s">
         <v>98</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F22" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>248308</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>100</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>101</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>102</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E23" t="s">
         <v>103</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>245501</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>105</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>106</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>107</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E24" t="s">
         <v>108</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F24" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>257022</v>
-      </c>
-      <c r="B24" t="s">
-        <v>110</v>
-      </c>
-      <c r="C24" t="s">
-        <v>111</v>
-      </c>
-      <c r="D24" t="s">
-        <v>112</v>
-      </c>
-      <c r="E24" t="s">
-        <v>113</v>
-      </c>
-      <c r="F24" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>253715</v>
       </c>
       <c r="B25" t="s">
         <v>110</v>
       </c>
       <c r="C25" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" t="s">
+        <v>112</v>
+      </c>
+      <c r="E25" t="s">
+        <v>113</v>
+      </c>
+      <c r="F25" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>253715</v>
+      </c>
+      <c r="B26" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" t="s">
         <v>115</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D26" t="s">
         <v>116</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E26" t="s">
         <v>117</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F26" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>140871</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>119</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>120</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>121</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E27" t="s">
         <v>122</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F27" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>253823</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>124</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>125</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" t="s">
         <v>126</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E28" t="s">
         <v>127</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F28" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>240673</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>129</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>130</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
         <v>131</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E29" t="s">
         <v>132</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F29" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>240849</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>134</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>135</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D30" t="s">
         <v>136</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E30" t="s">
         <v>137</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F30" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>258682</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>139</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>140</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D31" t="s">
         <v>141</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E31" t="s">
         <v>142</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F31" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>242851</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>144</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>145</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D32" t="s">
         <v>146</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E32" t="s">
         <v>147</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F32" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>246657</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>149</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>150</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>151</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E33" t="s">
         <v>152</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F33" t="s">
         <v>153</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>257854</v>
+      </c>
+      <c r="B34" t="s">
+        <v>164</v>
+      </c>
+      <c r="C34" t="s">
+        <v>165</v>
+      </c>
+      <c r="D34" t="s">
+        <v>166</v>
+      </c>
+      <c r="E34" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>236013</v>
+      </c>
+      <c r="B35" t="s">
+        <v>168</v>
+      </c>
+      <c r="C35" t="s">
+        <v>169</v>
+      </c>
+      <c r="D35" t="s">
+        <v>170</v>
+      </c>
+      <c r="E35" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>236866</v>
+      </c>
+      <c r="B36" t="s">
+        <v>172</v>
+      </c>
+      <c r="C36" t="s">
+        <v>173</v>
+      </c>
+      <c r="D36" t="s">
+        <v>174</v>
+      </c>
+      <c r="E36" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D17" r:id="rId1" xr:uid="{314B80AC-20EA-4C8F-883C-94CA0FC6FDE5}"/>
-    <hyperlink ref="D19" r:id="rId2" xr:uid="{88D29819-314C-493B-9B6F-BAEFCFC995AB}"/>
+    <hyperlink ref="D18" r:id="rId1" xr:uid="{314B80AC-20EA-4C8F-883C-94CA0FC6FDE5}"/>
+    <hyperlink ref="D20" r:id="rId2" xr:uid="{88D29819-314C-493B-9B6F-BAEFCFC995AB}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>